<commit_message>
Update BOM PMB Andromeda-V3.31.xlsx
</commit_message>
<xml_diff>
--- a/PowerManagementBoard_V3.31/BOM PMB Andromeda-V3.31.xlsx
+++ b/PowerManagementBoard_V3.31/BOM PMB Andromeda-V3.31.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noorg\OneDrive\Documents\GitHub\Andromeda-V3.3\PowerManagementBoard_V3.31\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3DEF60E-C763-4FA2-B079-E0E229E93BD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B6DD41-A629-4601-8FB7-2A1092C20DEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{BF07532D-72B4-43B2-830F-911E19F02528}"/>
   </bookViews>
@@ -316,10 +316,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -653,15 +653,16 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23.54296875" customWidth="1"/>
-    <col min="2" max="2" width="25.54296875" customWidth="1"/>
+    <col min="2" max="2" width="35.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.7265625" customWidth="1"/>
-    <col min="4" max="6" width="18.81640625" customWidth="1"/>
+    <col min="4" max="5" width="22.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -683,7 +684,7 @@
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="6" t="s">
         <v>69</v>
       </c>
     </row>
@@ -706,7 +707,7 @@
       <c r="F2" s="1">
         <v>3</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>71</v>
       </c>
     </row>
@@ -729,7 +730,7 @@
       <c r="F3" s="1">
         <v>2</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>71</v>
       </c>
     </row>
@@ -752,7 +753,7 @@
       <c r="F4" s="1">
         <v>2</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="5" t="s">
         <v>71</v>
       </c>
     </row>
@@ -775,7 +776,7 @@
       <c r="F5" s="1">
         <v>1</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="5" t="s">
         <v>71</v>
       </c>
     </row>
@@ -798,7 +799,7 @@
       <c r="F6" s="1">
         <v>1</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="5" t="s">
         <v>71</v>
       </c>
     </row>
@@ -821,7 +822,7 @@
       <c r="F7" s="1">
         <v>1</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="5" t="s">
         <v>71</v>
       </c>
     </row>
@@ -844,7 +845,7 @@
       <c r="F8" s="1">
         <v>3</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="5" t="s">
         <v>71</v>
       </c>
     </row>
@@ -867,7 +868,7 @@
       <c r="F9" s="1">
         <v>1</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="5" t="s">
         <v>71</v>
       </c>
     </row>
@@ -890,7 +891,7 @@
       <c r="F10" s="1">
         <v>1</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="5" t="s">
         <v>70</v>
       </c>
     </row>
@@ -913,7 +914,7 @@
       <c r="F11" s="1">
         <v>1</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="5" t="s">
         <v>71</v>
       </c>
     </row>
@@ -936,7 +937,7 @@
       <c r="F12" s="1">
         <v>2</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="5" t="s">
         <v>70</v>
       </c>
     </row>
@@ -959,7 +960,7 @@
       <c r="F13" s="1">
         <v>1</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="5" t="s">
         <v>70</v>
       </c>
     </row>
@@ -982,7 +983,7 @@
       <c r="F14" s="1">
         <v>1</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="5" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1005,7 +1006,7 @@
       <c r="F15" s="1">
         <v>1</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="5" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1028,7 +1029,7 @@
       <c r="F16" s="1">
         <v>2</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="5" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1051,7 +1052,7 @@
       <c r="F17" s="1">
         <v>1</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="5" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1074,7 +1075,7 @@
       <c r="F18" s="1">
         <v>1</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="G18" s="5" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1097,7 +1098,7 @@
       <c r="F19" s="1">
         <v>1</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="G19" s="5" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1120,7 +1121,7 @@
       <c r="F20" s="1">
         <v>1</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="G20" s="5" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1143,7 +1144,7 @@
       <c r="F21" s="1">
         <v>1</v>
       </c>
-      <c r="G21" s="6" t="s">
+      <c r="G21" s="5" t="s">
         <v>70</v>
       </c>
     </row>

</xml_diff>